<commit_message>
Y~1 analyses done for all tree sizes Y~X regression analyses done for all tree sizes
Added analyses comparing SAV to BWL in all pleths comparing Z scores using compare.z

Also looked at SAV in temperate vs tropical species and found significantly different levels of phylogenetic signal, tropical species having a kappa of 1.5, temp 0.5
</commit_message>
<xml_diff>
--- a/Literature_Review/1Summary.xlsx
+++ b/Literature_Review/1Summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericabaken/Documents/School/Projects/Lambda_Eval/Manuscript/2020-Adams_and_Baken/Literature_Review/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericabaken/Documents/School/Projects/2020-Adams_and_Baken/Literature_Review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37367CBD-5861-B449-A58B-4BF12A9506FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C32082-F604-024B-817D-4F4ABB292AE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="460" windowWidth="14660" windowHeight="17040" activeTab="1" xr2:uid="{A0FB5A63-E142-964D-A410-C63464937B8B}"/>
+    <workbookView xWindow="5540" yWindow="460" windowWidth="21360" windowHeight="17540" xr2:uid="{A0FB5A63-E142-964D-A410-C63464937B8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Since 2019" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5719" uniqueCount="1299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5719" uniqueCount="1300">
   <si>
     <t>Reference</t>
   </si>
@@ -3660,9 +3660,6 @@
     <t>Balsaminaceae</t>
   </si>
   <si>
-    <t>Yes, so bad "There was a marginally significant phylogenetic signal (λ = 0.54, 95 % CI 0.20–1.45)"</t>
-  </si>
-  <si>
     <t>Cited pagel 1999 when talking about doing pgls</t>
   </si>
   <si>
@@ -3760,12 +3757,6 @@
   </si>
   <si>
     <t>Kinda, not bad "The fact that the λ-value of 0.99 is very close to the maximum (λ = 1) means that the vascular area covaries in direct proportion with the species’ shared evolutionary history through a Brownian motion on the phylogeny [65,69]. "</t>
-  </si>
-  <si>
-    <t>Kinda, "we found that developmental variables exhibited strong phylogenetic signal, with λ values [95% CI]
-5
-bioRxiv preprint first posted online Oct. 8, 2019; doi: http://dx.doi.org/10.1101/797498. The copyright holder for this preprint (which was not peer-reviewed) is the author/funder, who has granted bioRxiv a license to display the preprint in perpetuity. It is made available under a CC-BY-NC 4.0 International license.
-165 of 0.93 [0.91, 0.94] and 0.86 [0.83, 0.89]"</t>
   </si>
   <si>
     <t>Kinda "PANCOVA estimated the phylogenetic signal as being quite large (λ = 0.9)"</t>
@@ -4240,6 +4231,15 @@
   </si>
   <si>
     <t>"[all analyses] were highly congruent with the molecular phylogenies"</t>
+  </si>
+  <si>
+    <t>No, interpreted well "There was a marginally significant phylogenetic signal (λ = 0.54, 95 % CI 0.20–1.45)"</t>
+  </si>
+  <si>
+    <t>Yes "phylogenetic signal (lambda = 0.65, 95 % CI 0.31-1.36) was high but not significantly different from zero)"</t>
+  </si>
+  <si>
+    <t>Kinda, "we found that developmental variables exhibited strong phylogenetic signal, with λ values [95% CI]  of 0.93 [0.91, 0.94] and 0.86 [0.83, 0.89]"</t>
   </si>
 </sst>
 </file>
@@ -4725,11 +4725,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5AD8032-AB13-4242-A1D6-BD5A6E1307B4}">
   <dimension ref="A1:M342"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:A1048576"/>
+      <selection pane="bottomRight" activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4771,7 +4771,7 @@
         <v>1117</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -4811,7 +4811,7 @@
         <v>154</v>
       </c>
       <c r="G3" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="H3" t="s">
         <v>891</v>
@@ -4855,7 +4855,7 @@
         <v>897</v>
       </c>
       <c r="M4" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -6428,7 +6428,7 @@
         <v>912</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="I64" s="2"/>
       <c r="J64" s="2" t="s">
@@ -6564,7 +6564,7 @@
         <v>903</v>
       </c>
       <c r="H71" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="J71" t="s">
         <v>896</v>
@@ -6590,7 +6590,7 @@
         <v>903</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>1241</v>
+        <v>1299</v>
       </c>
       <c r="I72" s="2"/>
       <c r="J72" t="s">
@@ -6755,7 +6755,7 @@
         <v>1009</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="I78" s="2"/>
       <c r="J78" s="2" t="s">
@@ -7536,7 +7536,7 @@
         <v>905</v>
       </c>
       <c r="H108" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="J108" t="s">
         <v>896</v>
@@ -8799,7 +8799,7 @@
         <v>1079</v>
       </c>
       <c r="H159" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="J159" t="s">
         <v>905</v>
@@ -9774,7 +9774,7 @@
         <v>903</v>
       </c>
       <c r="H198" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="J198" t="s">
         <v>905</v>
@@ -10378,7 +10378,7 @@
         <v>903</v>
       </c>
       <c r="H222" s="2" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="I222" s="2" t="s">
         <v>905</v>
@@ -10407,7 +10407,7 @@
         <v>905</v>
       </c>
       <c r="H223" s="2" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="I223" s="2"/>
       <c r="J223" s="2" t="s">
@@ -10608,7 +10608,7 @@
         <v>903</v>
       </c>
       <c r="H230" s="2" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="I230" s="2"/>
       <c r="J230" s="2" t="s">
@@ -10871,7 +10871,7 @@
         <v>1006</v>
       </c>
       <c r="H241" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="J241" t="s">
         <v>896</v>
@@ -12129,7 +12129,7 @@
         <v>1044</v>
       </c>
       <c r="F291" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="G291" t="s">
         <v>903</v>
@@ -12420,7 +12420,7 @@
         <v>903</v>
       </c>
       <c r="H303" t="s">
-        <v>1128</v>
+        <v>1298</v>
       </c>
       <c r="J303" t="s">
         <v>939</v>
@@ -12446,7 +12446,7 @@
         <v>903</v>
       </c>
       <c r="H304" t="s">
-        <v>1207</v>
+        <v>1297</v>
       </c>
       <c r="J304" t="s">
         <v>896</v>
@@ -12504,7 +12504,7 @@
         <v>964</v>
       </c>
       <c r="K306" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="307" spans="1:11">
@@ -12518,7 +12518,7 @@
         <v>156</v>
       </c>
       <c r="E307" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="F307">
         <v>5284</v>
@@ -12556,7 +12556,7 @@
         <v>903</v>
       </c>
       <c r="H308" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="J308" t="s">
         <v>896</v>
@@ -12582,7 +12582,7 @@
         <v>1057</v>
       </c>
       <c r="H309" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="J309" t="s">
         <v>896</v>
@@ -12610,7 +12610,7 @@
         <v>323</v>
       </c>
       <c r="E311" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="F311">
         <v>56</v>
@@ -12691,7 +12691,7 @@
         <v>556</v>
       </c>
       <c r="E314" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="F314">
         <v>1496</v>
@@ -12761,7 +12761,7 @@
         <v>896</v>
       </c>
       <c r="K316" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="317" spans="1:11">
@@ -12821,7 +12821,7 @@
         <v>1006</v>
       </c>
       <c r="H319" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="J319" t="s">
         <v>896</v>
@@ -12829,7 +12829,7 @@
     </row>
     <row r="320" spans="1:11">
       <c r="A320" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="C320" t="s">
         <v>650</v>
@@ -12838,7 +12838,7 @@
         <v>651</v>
       </c>
       <c r="E320" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="F320">
         <v>73</v>
@@ -12847,13 +12847,13 @@
         <v>1132</v>
       </c>
       <c r="H320" t="s">
+        <v>1215</v>
+      </c>
+      <c r="J320" t="s">
+        <v>896</v>
+      </c>
+      <c r="K320" t="s">
         <v>1216</v>
-      </c>
-      <c r="J320" t="s">
-        <v>896</v>
-      </c>
-      <c r="K320" t="s">
-        <v>1217</v>
       </c>
     </row>
     <row r="321" spans="1:11">
@@ -12899,7 +12899,7 @@
         <v>331</v>
       </c>
       <c r="E322" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="F322">
         <v>130</v>
@@ -12925,7 +12925,7 @@
         <v>233</v>
       </c>
       <c r="E323" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="F323">
         <v>452</v>
@@ -12954,7 +12954,7 @@
         <v>990</v>
       </c>
       <c r="F324" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="G324" t="s">
         <v>905</v>
@@ -12983,7 +12983,7 @@
         <v>10</v>
       </c>
       <c r="G325" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="H325" t="s">
         <v>896</v>
@@ -13018,7 +13018,7 @@
         <v>931</v>
       </c>
       <c r="K326" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="327" spans="1:11">
@@ -13052,7 +13052,7 @@
         <v>1006</v>
       </c>
       <c r="H328" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="J328" t="s">
         <v>896</v>
@@ -13069,7 +13069,7 @@
         <v>859</v>
       </c>
       <c r="E329" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="F329">
         <v>145</v>
@@ -13170,10 +13170,10 @@
         <v>11</v>
       </c>
       <c r="G333" t="s">
+        <v>1225</v>
+      </c>
+      <c r="H333" t="s">
         <v>1226</v>
-      </c>
-      <c r="H333" t="s">
-        <v>1227</v>
       </c>
       <c r="J333" t="s">
         <v>896</v>
@@ -13248,7 +13248,7 @@
         <v>31</v>
       </c>
       <c r="E336" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="F336">
         <v>765</v>
@@ -13309,7 +13309,7 @@
         <v>905</v>
       </c>
       <c r="H338" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="J338" t="s">
         <v>905</v>
@@ -13407,7 +13407,7 @@
         <v>931</v>
       </c>
       <c r="K342" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
   </sheetData>
@@ -13425,7 +13425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57F7C5C-7DCB-4F47-93C5-50E37A229EDB}">
   <dimension ref="A1:H1573"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+    <sheetView zoomScale="92" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -13447,20 +13447,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="1" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -13686,7 +13686,7 @@
         <v>1057</v>
       </c>
       <c r="G15" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -14608,7 +14608,7 @@
         <v>905</v>
       </c>
       <c r="G69" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -14662,7 +14662,7 @@
         <v>905</v>
       </c>
       <c r="G72" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -14682,7 +14682,7 @@
         <v>905</v>
       </c>
       <c r="G73" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -14719,7 +14719,7 @@
         <v>905</v>
       </c>
       <c r="G75" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -14892,7 +14892,7 @@
         <v>1057</v>
       </c>
       <c r="G85" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -14912,7 +14912,7 @@
         <v>905</v>
       </c>
       <c r="G86" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -14966,7 +14966,7 @@
         <v>1057</v>
       </c>
       <c r="G89" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -14986,7 +14986,7 @@
         <v>905</v>
       </c>
       <c r="G90" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -17487,7 +17487,7 @@
         <v>905</v>
       </c>
       <c r="G236" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="237" spans="1:7">
@@ -17507,7 +17507,7 @@
         <v>905</v>
       </c>
       <c r="G237" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="238" spans="1:7">
@@ -17527,7 +17527,7 @@
         <v>905</v>
       </c>
       <c r="G238" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="239" spans="1:7">
@@ -17702,7 +17702,7 @@
         <v>905</v>
       </c>
       <c r="G248" s="14" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="249" spans="1:8">
@@ -17723,7 +17723,7 @@
         <v>905</v>
       </c>
       <c r="G249" s="14" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="250" spans="1:8">
@@ -17762,10 +17762,10 @@
         <v>905</v>
       </c>
       <c r="G251" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="H251" s="14" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="252" spans="1:8">
@@ -18062,7 +18062,7 @@
         <v>905</v>
       </c>
       <c r="G268" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="269" spans="1:7">
@@ -18321,7 +18321,7 @@
         <v>905</v>
       </c>
       <c r="G283" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="284" spans="1:7">
@@ -18427,7 +18427,7 @@
         <v>905</v>
       </c>
       <c r="G289" s="15" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="290" spans="1:7">
@@ -18448,7 +18448,7 @@
         <v>905</v>
       </c>
       <c r="G290" s="15" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="291" spans="1:7">
@@ -18469,7 +18469,7 @@
         <v>905</v>
       </c>
       <c r="G291" s="15" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="292" spans="1:7">
@@ -18903,7 +18903,7 @@
         <v>905</v>
       </c>
       <c r="G316" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="317" spans="1:7">
@@ -18957,7 +18957,7 @@
         <v>905</v>
       </c>
       <c r="G319" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="320" spans="1:7">
@@ -18994,7 +18994,7 @@
         <v>905</v>
       </c>
       <c r="G321" s="9" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="322" spans="1:7">
@@ -19201,7 +19201,7 @@
         <v>905</v>
       </c>
       <c r="G333" s="2" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="334" spans="1:7">
@@ -19476,7 +19476,7 @@
         <v>1057</v>
       </c>
       <c r="G349" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="350" spans="1:7">
@@ -19751,7 +19751,7 @@
         <v>905</v>
       </c>
       <c r="G365" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="366" spans="1:7">
@@ -20061,7 +20061,7 @@
         <v>905</v>
       </c>
       <c r="G383" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="384" spans="1:7">
@@ -20837,7 +20837,7 @@
         <v>1057</v>
       </c>
       <c r="G428" s="2" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="429" spans="1:7">
@@ -20857,7 +20857,7 @@
         <v>1057</v>
       </c>
       <c r="G429" s="2" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="430" spans="1:7">
@@ -20877,7 +20877,7 @@
         <v>1057</v>
       </c>
       <c r="G430" s="2" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="431" spans="1:7">
@@ -21187,7 +21187,7 @@
         <v>905</v>
       </c>
       <c r="G448" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="449" spans="1:7">
@@ -21208,7 +21208,7 @@
         <v>905</v>
       </c>
       <c r="G449" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="450" spans="1:7">
@@ -21229,7 +21229,7 @@
         <v>905</v>
       </c>
       <c r="G450" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="451" spans="1:7">
@@ -21318,7 +21318,7 @@
         <v>905</v>
       </c>
       <c r="G455" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="456" spans="1:7">
@@ -21339,7 +21339,7 @@
         <v>905</v>
       </c>
       <c r="G456" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="457" spans="1:7">
@@ -21449,7 +21449,7 @@
         <v>484</v>
       </c>
       <c r="B463" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C463">
         <v>1E-4</v>
@@ -21483,7 +21483,7 @@
         <v>484</v>
       </c>
       <c r="B465" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C465">
         <v>1E-4</v>
@@ -21500,7 +21500,7 @@
         <v>484</v>
       </c>
       <c r="B466" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C466">
         <v>1E-4</v>
@@ -21568,7 +21568,7 @@
         <v>484</v>
       </c>
       <c r="B470" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C470">
         <v>1E-4</v>
@@ -21585,7 +21585,7 @@
         <v>484</v>
       </c>
       <c r="B471" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C471">
         <v>1E-4</v>
@@ -21602,7 +21602,7 @@
         <v>484</v>
       </c>
       <c r="B472" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C472">
         <v>1E-4</v>
@@ -21636,7 +21636,7 @@
         <v>484</v>
       </c>
       <c r="B474" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C474">
         <v>1E-4</v>
@@ -21653,7 +21653,7 @@
         <v>484</v>
       </c>
       <c r="B475" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C475">
         <v>1E-4</v>
@@ -21670,7 +21670,7 @@
         <v>484</v>
       </c>
       <c r="B476" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C476">
         <v>1E-4</v>
@@ -21687,7 +21687,7 @@
         <v>484</v>
       </c>
       <c r="B477" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C477">
         <v>1E-4</v>
@@ -21704,7 +21704,7 @@
         <v>484</v>
       </c>
       <c r="B478" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C478">
         <v>1E-4</v>
@@ -21721,7 +21721,7 @@
         <v>484</v>
       </c>
       <c r="B479" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C479">
         <v>1E-4</v>
@@ -21738,7 +21738,7 @@
         <v>484</v>
       </c>
       <c r="B480" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C480">
         <v>1E-4</v>
@@ -21755,7 +21755,7 @@
         <v>484</v>
       </c>
       <c r="B481" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C481">
         <v>1E-4</v>
@@ -21772,7 +21772,7 @@
         <v>484</v>
       </c>
       <c r="B482" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C482">
         <v>1E-4</v>
@@ -21789,7 +21789,7 @@
         <v>484</v>
       </c>
       <c r="B483" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C483">
         <v>1E-4</v>
@@ -21823,7 +21823,7 @@
         <v>484</v>
       </c>
       <c r="B485" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C485">
         <v>1E-4</v>
@@ -21840,7 +21840,7 @@
         <v>484</v>
       </c>
       <c r="B486" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C486">
         <v>1E-4</v>
@@ -21857,7 +21857,7 @@
         <v>484</v>
       </c>
       <c r="B487" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C487">
         <v>1E-4</v>
@@ -21874,7 +21874,7 @@
         <v>484</v>
       </c>
       <c r="B488" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C488">
         <v>1E-4</v>
@@ -21891,7 +21891,7 @@
         <v>484</v>
       </c>
       <c r="B489" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C489">
         <v>1E-4</v>
@@ -21908,7 +21908,7 @@
         <v>484</v>
       </c>
       <c r="B490" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C490">
         <v>1E-4</v>
@@ -21925,7 +21925,7 @@
         <v>484</v>
       </c>
       <c r="B491" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C491">
         <v>1E-4</v>
@@ -21942,7 +21942,7 @@
         <v>484</v>
       </c>
       <c r="B492" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C492">
         <v>1E-4</v>
@@ -22107,7 +22107,7 @@
         <v>905</v>
       </c>
       <c r="G501" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="502" spans="1:7">
@@ -23085,7 +23085,7 @@
         <v>905</v>
       </c>
       <c r="G558" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="559" spans="1:7">
@@ -26388,7 +26388,7 @@
         <v>905</v>
       </c>
       <c r="G752" s="16" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="753" spans="1:7">
@@ -26444,7 +26444,7 @@
         <v>905</v>
       </c>
       <c r="G755" s="17" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="756" spans="1:7">
@@ -26482,7 +26482,7 @@
         <v>905</v>
       </c>
       <c r="G757" s="17" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="758" spans="1:7">
@@ -26605,7 +26605,7 @@
         <v>905</v>
       </c>
       <c r="G764" s="17" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="765" spans="1:7">
@@ -26660,7 +26660,7 @@
         <v>905</v>
       </c>
       <c r="G767" s="17" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="768" spans="1:7">
@@ -26767,7 +26767,7 @@
         <v>905</v>
       </c>
       <c r="G773" s="17" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="774" spans="1:7">
@@ -26788,7 +26788,7 @@
         <v>905</v>
       </c>
       <c r="G774" s="17" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="775" spans="1:7">
@@ -26860,7 +26860,7 @@
         <v>905</v>
       </c>
       <c r="G778" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="779" spans="1:7">
@@ -28316,7 +28316,7 @@
         <v>905</v>
       </c>
       <c r="G863" s="18" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="864" spans="1:7">
@@ -29023,10 +29023,10 @@
         <v>905</v>
       </c>
       <c r="G903" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="H903" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="904" spans="1:8">
@@ -29047,7 +29047,7 @@
         <v>905</v>
       </c>
       <c r="G904" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="905" spans="1:8">
@@ -29068,7 +29068,7 @@
         <v>905</v>
       </c>
       <c r="G905" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="906" spans="1:8">
@@ -29089,7 +29089,7 @@
         <v>905</v>
       </c>
       <c r="G906" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="907" spans="1:8">
@@ -29417,7 +29417,7 @@
         <v>1057</v>
       </c>
       <c r="G925" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="926" spans="1:7">
@@ -29437,7 +29437,7 @@
         <v>905</v>
       </c>
       <c r="G926" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="927" spans="1:7">
@@ -29457,7 +29457,7 @@
         <v>905</v>
       </c>
       <c r="G927" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="928" spans="1:7">
@@ -29477,7 +29477,7 @@
         <v>905</v>
       </c>
       <c r="G928" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="929" spans="1:7">
@@ -29582,7 +29582,7 @@
         <v>905</v>
       </c>
       <c r="G934" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="935" spans="1:7">
@@ -30882,7 +30882,7 @@
         <v>1057</v>
       </c>
       <c r="G1010" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="1011" spans="1:7">
@@ -31504,7 +31504,7 @@
         <v>1057</v>
       </c>
       <c r="G1046" s="2" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="1047" spans="1:7">
@@ -31524,7 +31524,7 @@
         <v>1057</v>
       </c>
       <c r="G1047" s="2" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="1048" spans="1:7">
@@ -31544,7 +31544,7 @@
         <v>1057</v>
       </c>
       <c r="G1048" s="2" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="1049" spans="1:7">
@@ -31564,7 +31564,7 @@
         <v>1057</v>
       </c>
       <c r="G1049" s="2" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="1050" spans="1:7">
@@ -31638,7 +31638,7 @@
         <v>1057</v>
       </c>
       <c r="G1053" s="2" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="1054" spans="1:7">
@@ -32396,7 +32396,7 @@
         <v>1057</v>
       </c>
       <c r="G1097" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1098" spans="1:7">
@@ -32417,7 +32417,7 @@
         <v>1057</v>
       </c>
       <c r="G1098" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1099" spans="1:7">
@@ -32438,7 +32438,7 @@
         <v>1057</v>
       </c>
       <c r="G1099" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1100" spans="1:7">
@@ -32459,7 +32459,7 @@
         <v>1057</v>
       </c>
       <c r="G1100" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1101" spans="1:7">
@@ -32480,7 +32480,7 @@
         <v>1057</v>
       </c>
       <c r="G1101" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1102" spans="1:7">
@@ -32501,7 +32501,7 @@
         <v>1057</v>
       </c>
       <c r="G1102" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1103" spans="1:7">
@@ -32522,7 +32522,7 @@
         <v>1057</v>
       </c>
       <c r="G1103" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1104" spans="1:7">
@@ -32543,7 +32543,7 @@
         <v>1057</v>
       </c>
       <c r="G1104" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1105" spans="1:7">
@@ -32564,7 +32564,7 @@
         <v>1057</v>
       </c>
       <c r="G1105" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1106" spans="1:7">
@@ -32585,7 +32585,7 @@
         <v>1057</v>
       </c>
       <c r="G1106" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1107" spans="1:7">
@@ -32606,7 +32606,7 @@
         <v>1057</v>
       </c>
       <c r="G1107" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1108" spans="1:7">
@@ -32627,7 +32627,7 @@
         <v>1057</v>
       </c>
       <c r="G1108" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1109" spans="1:7">
@@ -32648,7 +32648,7 @@
         <v>1057</v>
       </c>
       <c r="G1109" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1110" spans="1:7">
@@ -32669,7 +32669,7 @@
         <v>1057</v>
       </c>
       <c r="G1110" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1111" spans="1:7">
@@ -32690,7 +32690,7 @@
         <v>1057</v>
       </c>
       <c r="G1111" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1112" spans="1:7">
@@ -32711,7 +32711,7 @@
         <v>1057</v>
       </c>
       <c r="G1112" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1113" spans="1:7">
@@ -32732,7 +32732,7 @@
         <v>1057</v>
       </c>
       <c r="G1113" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1114" spans="1:7">
@@ -32753,7 +32753,7 @@
         <v>1057</v>
       </c>
       <c r="G1114" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1115" spans="1:7">
@@ -32774,7 +32774,7 @@
         <v>1057</v>
       </c>
       <c r="G1115" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1116" spans="1:7">
@@ -32795,7 +32795,7 @@
         <v>1057</v>
       </c>
       <c r="G1116" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1117" spans="1:7">
@@ -32816,7 +32816,7 @@
         <v>1057</v>
       </c>
       <c r="G1117" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1118" spans="1:7">
@@ -32837,7 +32837,7 @@
         <v>1057</v>
       </c>
       <c r="G1118" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1119" spans="1:7">
@@ -32875,7 +32875,7 @@
         <v>1057</v>
       </c>
       <c r="G1120" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1121" spans="1:7">
@@ -32913,7 +32913,7 @@
         <v>1057</v>
       </c>
       <c r="G1122" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1123" spans="1:7">
@@ -32934,7 +32934,7 @@
         <v>1057</v>
       </c>
       <c r="G1123" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1124" spans="1:7">
@@ -34814,7 +34814,7 @@
         <v>1057</v>
       </c>
       <c r="G1233" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="1234" spans="1:7">
@@ -34834,7 +34834,7 @@
         <v>1057</v>
       </c>
       <c r="G1234" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="1235" spans="1:7">
@@ -34922,7 +34922,7 @@
         <v>1057</v>
       </c>
       <c r="G1239" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="1240" spans="1:7">
@@ -35690,7 +35690,7 @@
         <v>905</v>
       </c>
       <c r="G1284" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1285" spans="1:7">
@@ -35744,7 +35744,7 @@
         <v>905</v>
       </c>
       <c r="G1287" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1288" spans="1:7">
@@ -35798,7 +35798,7 @@
         <v>905</v>
       </c>
       <c r="G1290" s="9" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1291" spans="1:7">
@@ -35818,7 +35818,7 @@
         <v>905</v>
       </c>
       <c r="G1291" s="9" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1292" spans="1:7">
@@ -35838,7 +35838,7 @@
         <v>905</v>
       </c>
       <c r="G1292" s="9" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1293" spans="1:7">
@@ -35909,7 +35909,7 @@
         <v>905</v>
       </c>
       <c r="G1296" s="9" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1297" spans="1:7">
@@ -35929,7 +35929,7 @@
         <v>905</v>
       </c>
       <c r="G1297" s="9" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1298" spans="1:7">
@@ -35966,7 +35966,7 @@
         <v>905</v>
       </c>
       <c r="G1299" s="9" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1300" spans="1:7">
@@ -36003,7 +36003,7 @@
         <v>905</v>
       </c>
       <c r="G1301" s="9" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1302" spans="1:7">
@@ -36601,7 +36601,7 @@
         <v>905</v>
       </c>
       <c r="G1336" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="1337" spans="1:7">
@@ -37574,7 +37574,7 @@
         <v>905</v>
       </c>
       <c r="G1393" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="1394" spans="1:7">
@@ -37595,7 +37595,7 @@
         <v>905</v>
       </c>
       <c r="G1394" s="12" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="1395" spans="1:7">
@@ -38616,7 +38616,7 @@
         <v>905</v>
       </c>
       <c r="G1453" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1454" spans="1:7">
@@ -38636,7 +38636,7 @@
         <v>905</v>
       </c>
       <c r="G1454" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1455" spans="1:7">
@@ -38656,7 +38656,7 @@
         <v>905</v>
       </c>
       <c r="G1455" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1456" spans="1:7">
@@ -38710,7 +38710,7 @@
         <v>905</v>
       </c>
       <c r="G1458" s="9" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1459" spans="1:7">
@@ -38747,7 +38747,7 @@
         <v>905</v>
       </c>
       <c r="G1460" s="9" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1461" spans="1:7">
@@ -38767,7 +38767,7 @@
         <v>905</v>
       </c>
       <c r="G1461" s="9" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1462" spans="1:7">
@@ -38787,7 +38787,7 @@
         <v>905</v>
       </c>
       <c r="G1462" s="9" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1463" spans="1:7">
@@ -38807,7 +38807,7 @@
         <v>905</v>
       </c>
       <c r="G1463" s="9" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1464" spans="1:7">
@@ -38878,7 +38878,7 @@
         <v>905</v>
       </c>
       <c r="G1467" s="9" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1468" spans="1:7">
@@ -39580,7 +39580,7 @@
     </row>
     <row r="1509" spans="1:8">
       <c r="A1509" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B1509">
         <v>0.82</v>
@@ -39595,12 +39595,12 @@
         <v>905</v>
       </c>
       <c r="G1509" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="1510" spans="1:8">
       <c r="A1510" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B1510">
         <v>0.34</v>
@@ -39615,12 +39615,12 @@
         <v>1057</v>
       </c>
       <c r="G1510" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="1511" spans="1:8">
       <c r="A1511" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B1511">
         <v>0.41</v>
@@ -39635,7 +39635,7 @@
         <v>905</v>
       </c>
       <c r="G1511" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="1512" spans="1:8">
@@ -39710,10 +39710,10 @@
         <v>905</v>
       </c>
       <c r="G1515" s="19" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="H1515" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="1516" spans="1:8">
@@ -39770,7 +39770,7 @@
         <v>905</v>
       </c>
       <c r="G1518" s="19" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1519" spans="1:8">
@@ -39791,7 +39791,7 @@
         <v>905</v>
       </c>
       <c r="G1519" s="19" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1520" spans="1:8">
@@ -39812,7 +39812,7 @@
         <v>905</v>
       </c>
       <c r="G1520" s="19" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1521" spans="1:6">
@@ -40563,7 +40563,7 @@
         <v>905</v>
       </c>
       <c r="G1564" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="1565" spans="1:7">
@@ -40689,7 +40689,7 @@
         <v>905</v>
       </c>
       <c r="G1571" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="1572" spans="1:7">

</xml_diff>

<commit_message>
Editing figures to use $\kappa$ instead of K
</commit_message>
<xml_diff>
--- a/Literature_Review/1Summary.xlsx
+++ b/Literature_Review/1Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericabaken/Documents/School/Projects/2020-Adams_and_Baken/Literature_Review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C32082-F604-024B-817D-4F4ABB292AE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096EDBD1-7500-4648-A14C-2868205BF680}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="460" windowWidth="21360" windowHeight="17540" xr2:uid="{A0FB5A63-E142-964D-A410-C63464937B8B}"/>
+    <workbookView xWindow="5540" yWindow="460" windowWidth="21360" windowHeight="17540" activeTab="1" xr2:uid="{A0FB5A63-E142-964D-A410-C63464937B8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Since 2019" sheetId="1" r:id="rId1"/>
@@ -4725,7 +4725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5AD8032-AB13-4242-A1D6-BD5A6E1307B4}">
   <dimension ref="A1:M342"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -13425,20 +13425,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57F7C5C-7DCB-4F47-93C5-50E37A229EDB}">
   <dimension ref="A1:H1573"/>
   <sheetViews>
-    <sheetView zoomScale="92" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12:A14"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="25.5" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="3.5" style="6" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="6" customWidth="1"/>
     <col min="6" max="6" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13579,7 +13579,9 @@
       <c r="C8" s="12">
         <v>0.96</v>
       </c>
-      <c r="D8" s="12"/>
+      <c r="D8" s="12">
+        <v>154</v>
+      </c>
       <c r="E8" s="13"/>
       <c r="F8" s="12" t="s">
         <v>896</v>
@@ -13593,7 +13595,9 @@
       <c r="C9" s="12">
         <v>0.65</v>
       </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="12">
+        <v>154</v>
+      </c>
       <c r="E9" s="13"/>
       <c r="F9" s="12" t="s">
         <v>896</v>
@@ -13607,7 +13611,9 @@
       <c r="C10" s="12">
         <v>0.82</v>
       </c>
-      <c r="D10" s="12"/>
+      <c r="D10" s="12">
+        <v>154</v>
+      </c>
       <c r="E10" s="13"/>
       <c r="F10" s="12" t="s">
         <v>896</v>
@@ -13621,7 +13627,9 @@
       <c r="C11" s="12">
         <v>0.77</v>
       </c>
-      <c r="D11" s="12"/>
+      <c r="D11" s="12">
+        <v>154</v>
+      </c>
       <c r="E11" s="13"/>
       <c r="F11" s="12" t="s">
         <v>896</v>
@@ -13635,7 +13643,9 @@
       <c r="C12" s="12">
         <v>0.71</v>
       </c>
-      <c r="D12" s="12"/>
+      <c r="D12" s="12">
+        <v>154</v>
+      </c>
       <c r="E12" s="13"/>
       <c r="F12" s="12" t="s">
         <v>896</v>
@@ -13649,7 +13659,9 @@
       <c r="C13" s="12">
         <v>0</v>
       </c>
-      <c r="D13" s="12"/>
+      <c r="D13" s="12">
+        <v>154</v>
+      </c>
       <c r="E13" s="13"/>
       <c r="F13" s="12" t="s">
         <v>896</v>
@@ -13663,7 +13675,9 @@
       <c r="C14" s="12">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D14" s="12"/>
+      <c r="D14" s="12">
+        <v>154</v>
+      </c>
       <c r="E14" s="13"/>
       <c r="F14" s="12" t="s">
         <v>896</v>

</xml_diff>